<commit_message>
tabella dati elevato valore
</commit_message>
<xml_diff>
--- a/risorse/dati-elevato-valore.xlsx
+++ b/risorse/dati-elevato-valore.xlsx
@@ -2,13 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="geospaziali" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="terra_ambiente" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="meteorologici" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="statistici" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="imprese" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="mobilita" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="40">
   <si>
     <t xml:space="preserve">Categoria tematica</t>
   </si>
@@ -174,6 +180,52 @@
   </si>
   <si>
     <t xml:space="preserve">I metadati che descrivono le serie di dati sulle reti di trasporto contengono almeno gli elementi di metadati definiti nel Regolamento (CE) n. 1205/2008.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le serie di dati sono messe a disposizione per il riutilizzo: 
+- alle condizioni della licenza Creative Commons BY 4.0 o di una licenza aperta equivalente o meno restrittiva; 
+- in un formato aperto leggibile meccanicamente, pubblicamente 
+documentato e riconosciuto dall’Unione o a livello internazionale; 
+- tramite interfacce di programmazione delle applicazioni ("API") e download in blocco; 
+- [nella versione più aggiornata].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le serie di dati sono messe a disposizione per il riutilizzo: 
+- alle condizioni della licenza Creative Commons BY 4.0 o di una licenza aperta equivalente o meno restrittiva; 
+- in un formato aperto leggibile meccanicamente, pubblicamente documentato e riconosciuto dall’Unione o a livello internazionale; 
+- tramite API e download in blocco (per le versioni storiche delle serie di dati: API o download in blocco, per quanto possibile e opportuno).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le serie di dati sono messe a disposizione per il riutilizzo: 
+- alle condizioni della licenza Creative Commons BY 4.0 o di una licenza aperta equivalente o meno restrittiva; 
+- in uno qualsiasi dei formati specificati nella tabella presente al par. 3.2 dell’Allegato I o in un altro formato aperto, leggibile meccanicamente, riconosciuto dall’Unione o a livello internazionale; 
+- tramite API e download in blocco, ad eccezione della serie di dati «dati dei modelli NWP», che è resa disponibile solo tramite API; 
+- [in base alla frequenza e alla tempestività di aggiornamento specificate nella tabella presente nel par. 3.2 dell’Allegato I].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le serie di dati sono messe a disposizione per il riutilizzo: 
+- [con la frequenza richiesta dalla legislazione corrispondente di cui al punto 4.1. dell’Allegato I (ad es. mensile, trimestrale, annuale)]; 
+- alle condizioni della licenza Creative Commons BY 4.0 o di una licenza aperta equivalente o meno restrittiva; 
+- in un formato CSV, XML (SDMX), JSON o in altro formato aperto leggibile meccanicamente, pubblicamente documentato e riconosciuto dall’Unione o a livello internazionale;
+- tramite API e download in blocco;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le serie di dati sono messe a disposizione per il riutilizzo: 
+- [senza indebito ritardo dopo l'ultimo aggiornamento]; 
+- alle condizioni della licenza Creative Commons BY 4.0 o di una licenza aperta equivalente o meno restrittiva, con condizioni supplementari relative al riutilizzo dei dati personali, se del caso; 
+- in un formato aperto leggibile meccanicamente e riconosciuto 
+dall’Unione o a livello internazionale (XHTML per i documenti che 
+rientrano nell’ambito di applicazione del Regolamento Delegato (UE) 2018/815 della Commissione; altri formati, se e ove prescritto dal diritto dell'Unione applicabile), con metadati completi ([per i documenti che rientrano nell’ambito di applicazione del Regolamento Delegato (UE) 2016/1437 della Commissione, i metadati specificati in tale regolamento, se del caso;] per gli altri documenti, i metadati prescritti dal diritto dell’UE applicabile, se del caso); la leggibilità meccanica non è imposta per i dati conservati in formati non leggibili meccanicamente (ad es. documenti e conti aziendali scannerizzati) o per I campi di dati non strutturati/non leggibili meccanicamente inclusi come parte di documenti leggibili meccanicamente; 
+- tramite API e download in blocco; 
+- [a livello di singola azienda].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le serie di dati della rete di trasporto sono messe a disposizione per il riutilizzo
+- [immediatamente dopo l’ultimo aggiornamento]; 
+- alle condizioni della licenza Creative Commons BY 4.0 o di una licenza aperta equivalente o meno restrittiva; 
+- in un formato aperto leggibile meccanicamente e riconosciuto dall’Unione o a livello internazionale;
+- tramite API e download in blocco;
+- [nella versione più aggiornata].</t>
   </si>
 </sst>
 </file>
@@ -272,20 +324,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,13 +536,13 @@
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="A:C"/>
+      <selection pane="bottomLeft" activeCell="C1" activeCellId="1" sqref="A1:B5 C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="50.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -500,203 +556,203 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="108.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="283.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="122.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
-      <c r="B20" s="3" t="s">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
-      <c r="B21" s="3" t="s">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -717,4 +773,394 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="50.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="50.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="50.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="50.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="50.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="283.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="50.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="122.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>